<commit_message>
splits each sentence into array of words
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
           <t>sentences</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>word</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -449,6 +454,11 @@
           <t>Colonialism in the Americas is a complex and multifaceted topic that has shaped the history culture and identity of the region</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['Colonialism', 'in', 'the', 'Americas', 'is', 'a', 'complex', 'and', 'multifaceted', 'topic', 'that', 'has', 'shaped', 'the', 'history', 'culture', 'and', 'identity', 'of', 'the', 'region']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -459,6 +469,11 @@
           <t>From the arrival of Christopher Columbus in 1492 European powers established colonies throughout the Americas with the aim of extracting resources spreading Christianity and asserting their dominance over the land and people</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['From', 'the', 'arrival', 'of', 'Christopher', 'Columbus', 'in', '1492', 'European', 'powers', 'established', 'colonies', 'throughout', 'the', 'Americas', 'with', 'the', 'aim', 'of', 'extracting', 'resources', 'spreading', 'Christianity', 'and', 'asserting', 'their', 'dominance', 'over', 'the', 'land', 'and', 'people']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -469,6 +484,11 @@
           <t>The impact of colonialism in the Americas was far-reaching both positive and negative</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['The', 'impact', 'of', 'colonialism', 'in', 'the', 'Americas', 'was', 'far-reaching', 'both', 'positive', 'and', 'negative']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -479,6 +499,11 @@
           <t>On one hand the arrival of Europeans brought new technologies ideas and institutions to the region</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['On', 'one', 'hand', 'the', 'arrival', 'of', 'Europeans', 'brought', 'new', 'technologies', 'ideas', 'and', 'institutions', 'to', 'the', 'region']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -489,6 +514,11 @@
           <t>The introduction of crops such as wheat sugarcane and tobacco revolutionized agriculture and created new economic opportunities for both Europeans and indigenous peoples</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['The', 'introduction', 'of', 'crops', 'such', 'as', 'wheat', 'sugarcane', 'and', 'tobacco', 'revolutionized', 'agriculture', 'and', 'created', 'new', 'economic', 'opportunities', 'for', 'both', 'Europeans', 'and', 'indigenous', 'peoples']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -499,6 +529,11 @@
           <t>Christianity and other religions also spread throughout the region leading to the construction of impressive cathedrals and the establishment of religious orders that provided education and healthcare</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['Christianity', 'and', 'other', 'religions', 'also', 'spread', 'throughout', 'the', 'region', 'leading', 'to', 'the', 'construction', 'of', 'impressive', 'cathedrals', 'and', 'the', 'establishment', 'of', 'religious', 'orders', 'that', 'provided', 'education', 'and', 'healthcare']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -509,6 +544,11 @@
           <t>However the benefits of colonialism were not shared equally</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['However', 'the', 'benefits', 'of', 'colonialism', 'were', 'not', 'shared', 'equally']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -519,6 +559,11 @@
           <t>European colonizers imposed their own systems of government law and economy onto the region often at the expense of indigenous peoples</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['European', 'colonizers', 'imposed', 'their', 'own', 'systems', 'of', 'government', 'law', 'and', 'economy', 'onto', 'the', 'region', 'often', 'at', 'the', 'expense', 'of', 'indigenous', 'peoples']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -529,6 +574,11 @@
           <t>The exploitation of resources such as gold silver and other minerals led to environmental degradation and economic instability</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['The', 'exploitation', 'of', 'resources', 'such', 'as', 'gold', 'silver', 'and', 'other', 'minerals', 'led', 'to', 'environmental', 'degradation', 'and', 'economic', 'instability']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -539,94 +589,9 @@
           <t>The forced labor of enslaved Africans and indigenous peoples contributed to the growth of the Atlantic slave trade and the creation of racial hierarchies that persist to this day</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Colonialism in the Americas also had a profound impact on culture and identity</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>European powers imposed their own languages customs and beliefs onto the region often leading to the erasure of indigenous cultures and the creation of new hybrid cultures</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Indigenous peoples were forced to assimilate to European ways of life often through violent means leading to the loss of traditional knowledge languages and practices</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Despite the negative impacts of colonialism the Americas have emerged as a vibrant and diverse region with a rich cultural heritage</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>The struggle for independence from European powers in the 19th and 20th centuries led to the creation of new nations and the emergence of new political economic and cultural movements</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Indigenous peoples have also been at the forefront of social and political change fighting for recognition of their rights lands and cultures</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>In conclusion colonialism in the Americas is a complex and nuanced topic that continues to shape the region to this day</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>While the legacy of colonialism has had many negative impacts it has also contributed to the creation of new cultures ideas and institutions</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Understanding the history of colonialism is crucial for understanding the challenges and opportunities facing the region in the present and future</t>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['The', 'forced', 'labor', 'of', 'enslaved', 'Africans', 'and', 'indigenous', 'peoples', 'contributed', 'to', 'the', 'growth', 'of', 'the', 'Atlantic', 'slave', 'trade', 'and', 'the', 'creation', 'of', 'racial', 'hierarchies', 'that', 'persist', 'to', 'this', 'day']</t>
         </is>
       </c>
     </row>

</xml_diff>